<commit_message>
updated the data transfer methods section
</commit_message>
<xml_diff>
--- a/draft/figure/Graph/not_realtask/xls/Memcpy_cpuload_DtoH.xlsx
+++ b/draft/figure/Graph/not_realtask/xls/Memcpy_cpuload_DtoH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="-440" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DMA" sheetId="9" r:id="rId1"/>
@@ -15,6 +15,9 @@
     <sheet name="GPC4" sheetId="14" r:id="rId6"/>
     <sheet name="グラフ" sheetId="7" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1487,11 +1490,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117387928"/>
-        <c:axId val="2117393688"/>
+        <c:axId val="2094605224"/>
+        <c:axId val="2123561576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117387928"/>
+        <c:axId val="2094605224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1530,7 +1533,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117393688"/>
+        <c:crossAx val="2123561576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1539,7 +1542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117393688"/>
+        <c:axId val="2123561576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1569,7 +1572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117387928"/>
+        <c:crossAx val="2094605224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3614,11 +3617,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2075002568"/>
-        <c:axId val="2117433288"/>
+        <c:axId val="2094580344"/>
+        <c:axId val="2043303528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2075002568"/>
+        <c:axId val="2094580344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3657,7 +3660,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117433288"/>
+        <c:crossAx val="2043303528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3666,7 +3669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117433288"/>
+        <c:axId val="2043303528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20.0"/>
@@ -3697,7 +3700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075002568"/>
+        <c:crossAx val="2094580344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4800,11 +4803,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115248888"/>
-        <c:axId val="2115254632"/>
+        <c:axId val="2094639944"/>
+        <c:axId val="2086134744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2115248888"/>
+        <c:axId val="2094639944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4843,7 +4846,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115254632"/>
+        <c:crossAx val="2086134744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -4852,7 +4855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115254632"/>
+        <c:axId val="2086134744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20.0"/>
@@ -4883,7 +4886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115248888"/>
+        <c:crossAx val="2094639944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6852,11 +6855,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2075097080"/>
-        <c:axId val="2074926600"/>
+        <c:axId val="2125617944"/>
+        <c:axId val="2130095816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2075097080"/>
+        <c:axId val="2125617944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6896,7 +6899,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2074926600"/>
+        <c:crossAx val="2130095816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -6905,7 +6908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074926600"/>
+        <c:axId val="2130095816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20.0"/>
@@ -6937,7 +6940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075097080"/>
+        <c:crossAx val="2125617944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8005,11 +8008,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127751304"/>
-        <c:axId val="2127757064"/>
+        <c:axId val="2134256824"/>
+        <c:axId val="2134262584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127751304"/>
+        <c:axId val="2134256824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8049,7 +8052,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127757064"/>
+        <c:crossAx val="2134262584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -8058,7 +8061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127757064"/>
+        <c:axId val="2134262584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -8091,7 +8094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127751304"/>
+        <c:crossAx val="2134256824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9166,11 +9169,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127806664"/>
-        <c:axId val="2127812424"/>
+        <c:axId val="2134312808"/>
+        <c:axId val="2134318568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127806664"/>
+        <c:axId val="2134312808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9210,7 +9213,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127812424"/>
+        <c:crossAx val="2134318568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9219,7 +9222,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127812424"/>
+        <c:axId val="2134318568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -9252,7 +9255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127806664"/>
+        <c:crossAx val="2134312808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9293,6 +9296,2366 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.106917565399112"/>
+          <c:y val="0.0557551475024364"/>
+          <c:w val="0.85385509571967"/>
+          <c:h val="0.775684760917655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>DMA</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DMA!$B$7:$X$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>90.00099899999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.00099899999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.00599699999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.00099899999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.00299800000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.001999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.00099899999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.001999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.00299800000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.027</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90.00599699999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90.014999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90.018997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>90.03600299999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90.03600299999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90.03600299999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90.03600299999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90.011002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90.66799899999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>270.502991</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>640.002014</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1270.105957</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>IORW</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>IORW!$B$7:$X$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.022</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.041</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>189.449997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>379.389008</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>389.268005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>679.10498</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1159.699951</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1489.999023</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1059.458008</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1199.487061</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1479.389038</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>489.006012</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>680.000977</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1350.000977</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2690.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5374.165039</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MEMWND</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PMEM!$B$7:$T$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.018</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.052</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.084</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.148</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131.013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210.388</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>499.838989</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>960.117981</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1920.170044</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4030.227051</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8240.116211</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16730.677734</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>HUB</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HUB!$B$7:$X$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.015</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.024</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.037</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.062</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.208</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89.112999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>129.345001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94.66999800000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.386002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>579.744019</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>121.404999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>889.106995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>219.005997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>190.882996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210.839005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>381.466003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>GPC1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GPC!$B$7:$X$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.021</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.028</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.041</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.103</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.126</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.235</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89.096001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90.001999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>159.998993</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100.000999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>779.997009</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>890.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1020.000977</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>989.999023</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>125.530998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>700.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>GPC4</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'GPC4'!$B$7:$X$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.022</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.027</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.036</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.053</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.088</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.303</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.585</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>91.39299800000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>89.785004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99.566002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.934998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>109.205002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>899.726013</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>162.395996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>159.164001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2122744008"/>
+        <c:axId val="2121923272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2122744008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>Data Size </a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" sz="2400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-1080000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2200"/>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2121923272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="0"/>
+        <c:tickLblSkip val="2"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2121923272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>Data Transfer Time ( ms )</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" sz="2400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2200"/>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2122744008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.112490390715379"/>
+          <c:y val="0.0809147162105719"/>
+          <c:w val="0.149332387953875"/>
+          <c:h val="0.300541280571756"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.106917565399112"/>
+          <c:y val="0.0557551475024364"/>
+          <c:w val="0.85385509571967"/>
+          <c:h val="0.775684760917655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>DMA</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DMA!$B$9:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>72.99442973999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.07379955999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.11539969999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.99544954999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.25220942999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.08386927999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.21083920999991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.95025917999991</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.21785916999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.44757904</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.00281842999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84.56625753000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84.28407245000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.73951797</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.7641894300001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>61.54874925000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>72.93373841000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30.31955946999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.75124032</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>86.2400901900001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>252.1304705299999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>574.3844766299998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1033.10393584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>IORW</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>IORW!$B$9:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.00321</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00446</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01116</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02089</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.04002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0786</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15547</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.30941</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104.2466898</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>116.3330997000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>117.44287039</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>129.15336993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.86484940999994</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>665.0127410399998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80.48370009000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>106.77131053</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>199.4265814100001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>339.0204598699999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>670.0258277300003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1338.88741706</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2676.78968266</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5351.504238399998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MEMWND</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PMEM!$B$9:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.00573</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0064</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00751</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01551</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.02587</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.07549</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.40039</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.075730000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.953729999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.840210000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>102.1002789500001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>206.06519874</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>412.06307167</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>790.0021015100002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1661.802347450001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3769.09177248</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8122.434140640002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13688.57188417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>HUB</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HUB!$B$9:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.01245</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01212</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01213</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01385</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01746</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02283</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.035</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.05941</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10822</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.20594</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.288419989999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.77834128999986</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.43344917000013</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>79.96037061000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>71.51511989999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>79.79617026000008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.96247965999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>85.17954962999994</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>110.00261976</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>204.46239013</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>378.7927780100001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>GPC1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GPC!$B$9:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.01573</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01517</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01541</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18236</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01534</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01708</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.02073</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.04003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0687299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12321</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.23319</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82.08754179999987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>77.26100011000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>83.24444015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>79.30581027000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>141.46844987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>122.58890109</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>138.12205008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>137.36729996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>123.02953938</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>247.1824399000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>493.8084407000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>GPC4</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>DMA!$B$5:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>16 B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32 B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64 B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128 B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256 B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512 B</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1 KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2 KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4 KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8 KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16 KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32 KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64 KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128 KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256 KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512 KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2 MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4 MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8 MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16 MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32 MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'GPC4'!$B$9:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.01742</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01726</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01748</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01733</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01731</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01735</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0209</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.02469</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0333999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.05196</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0870999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15815</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29914</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58068</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>86.03068757000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87.92566773000013</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85.04548143000007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>81.63947880999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>84.06103979000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>78.31171993000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>88.04850043000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>159.1585905899997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2120709448"/>
+        <c:axId val="2121235928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2120709448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>Data Size </a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" sz="2400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-1080000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2200"/>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2121235928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="0"/>
+        <c:tickLblSkip val="2"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2121235928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>Data Transfer Time ( ms )</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" sz="2400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2200"/>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2120709448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.112490390715379"/>
+          <c:y val="0.316671101279334"/>
+          <c:w val="0.149332387953875"/>
+          <c:h val="0.300541280571756"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="ja-JP"/>
     </a:p>
@@ -9499,7 +11862,581 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="グラフ 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="グラフ 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="DMA"/>
+      <sheetName val="IORW"/>
+      <sheetName val="PMEM"/>
+      <sheetName val="HUB"/>
+      <sheetName val="GPC"/>
+      <sheetName val="GPC4"/>
+      <sheetName val="グラフ"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>16 B</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>32 B</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>64 B</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>128 B</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>256 B</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>512 B</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>1 KB</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>2 KB</v>
+          </cell>
+          <cell r="J5" t="str">
+            <v>4 KB</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>8 KB</v>
+          </cell>
+          <cell r="L5" t="str">
+            <v>16 KB</v>
+          </cell>
+          <cell r="M5" t="str">
+            <v>32 KB</v>
+          </cell>
+          <cell r="N5" t="str">
+            <v>64 KB</v>
+          </cell>
+          <cell r="O5" t="str">
+            <v>128 KB</v>
+          </cell>
+          <cell r="P5" t="str">
+            <v>256 KB</v>
+          </cell>
+          <cell r="Q5" t="str">
+            <v>512 KB</v>
+          </cell>
+          <cell r="R5" t="str">
+            <v>1 MB</v>
+          </cell>
+          <cell r="S5" t="str">
+            <v>2 MB</v>
+          </cell>
+          <cell r="T5" t="str">
+            <v>4 MB</v>
+          </cell>
+          <cell r="U5" t="str">
+            <v>8 MB</v>
+          </cell>
+          <cell r="V5" t="str">
+            <v>16 MB</v>
+          </cell>
+          <cell r="W5" t="str">
+            <v>32 MB</v>
+          </cell>
+          <cell r="X5" t="str">
+            <v>64 MB</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>0.50439000000000012</v>
+          </cell>
+          <cell r="C9">
+            <v>0.56759999999999977</v>
+          </cell>
+          <cell r="D9">
+            <v>0.51110000000000022</v>
+          </cell>
+          <cell r="E9">
+            <v>0.53892999999999991</v>
+          </cell>
+          <cell r="F9">
+            <v>0.50746999999999987</v>
+          </cell>
+          <cell r="G9">
+            <v>0.52881000000000011</v>
+          </cell>
+          <cell r="H9">
+            <v>0.49443999999999988</v>
+          </cell>
+          <cell r="I9">
+            <v>0.53405000000000002</v>
+          </cell>
+          <cell r="J9">
+            <v>0.53729000000000005</v>
+          </cell>
+          <cell r="K9">
+            <v>0.59913999999999989</v>
+          </cell>
+          <cell r="L9">
+            <v>0.57677000000000012</v>
+          </cell>
+          <cell r="M9">
+            <v>0.63575000000000026</v>
+          </cell>
+          <cell r="N9">
+            <v>0.63066999999999995</v>
+          </cell>
+          <cell r="O9">
+            <v>0.60153999999999996</v>
+          </cell>
+          <cell r="P9">
+            <v>0.59076000000000006</v>
+          </cell>
+          <cell r="Q9">
+            <v>0.64145000000000008</v>
+          </cell>
+          <cell r="R9">
+            <v>0.69660000000000011</v>
+          </cell>
+          <cell r="S9">
+            <v>0.86072000000000015</v>
+          </cell>
+          <cell r="T9">
+            <v>1.1444600000000005</v>
+          </cell>
+          <cell r="U9">
+            <v>1.81203</v>
+          </cell>
+          <cell r="V9">
+            <v>3.0765699999999976</v>
+          </cell>
+          <cell r="W9">
+            <v>5.6455799999999998</v>
+          </cell>
+          <cell r="X9">
+            <v>10.701120000000003</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="9">
+          <cell r="B9">
+            <v>5.2200000000000033E-3</v>
+          </cell>
+          <cell r="C9">
+            <v>5.2700000000000038E-3</v>
+          </cell>
+          <cell r="D9">
+            <v>4.9800000000000035E-3</v>
+          </cell>
+          <cell r="E9">
+            <v>4.7900000000000035E-3</v>
+          </cell>
+          <cell r="F9">
+            <v>4.9300000000000038E-3</v>
+          </cell>
+          <cell r="G9">
+            <v>5.0400000000000037E-3</v>
+          </cell>
+          <cell r="H9">
+            <v>5.2400000000000033E-3</v>
+          </cell>
+          <cell r="I9">
+            <v>5.4300000000000034E-3</v>
+          </cell>
+          <cell r="J9">
+            <v>5.7300000000000042E-3</v>
+          </cell>
+          <cell r="K9">
+            <v>6.6600000000000036E-3</v>
+          </cell>
+          <cell r="L9">
+            <v>8.2200000000000068E-3</v>
+          </cell>
+          <cell r="M9">
+            <v>1.3349999999999994E-2</v>
+          </cell>
+          <cell r="N9">
+            <v>2.0759999999999983E-2</v>
+          </cell>
+          <cell r="O9">
+            <v>3.6059999999999974E-2</v>
+          </cell>
+          <cell r="P9">
+            <v>6.6920000000000007E-2</v>
+          </cell>
+          <cell r="Q9">
+            <v>0.12551000000000001</v>
+          </cell>
+          <cell r="R9">
+            <v>0.23211999999999999</v>
+          </cell>
+          <cell r="S9">
+            <v>0.45490999999999993</v>
+          </cell>
+          <cell r="T9">
+            <v>0.92941000000000018</v>
+          </cell>
+          <cell r="U9">
+            <v>1.8752099999999994</v>
+          </cell>
+          <cell r="V9">
+            <v>3.7371900000000009</v>
+          </cell>
+          <cell r="W9">
+            <v>7.4926600000000017</v>
+          </cell>
+          <cell r="X9">
+            <v>14.880720000000002</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="9">
+          <cell r="B9">
+            <v>2.8060000000000015E-2</v>
+          </cell>
+          <cell r="C9">
+            <v>2.7830000000000008E-2</v>
+          </cell>
+          <cell r="D9">
+            <v>2.6989999999999979E-2</v>
+          </cell>
+          <cell r="E9">
+            <v>1.8099999999999984E-2</v>
+          </cell>
+          <cell r="F9">
+            <v>2.8789999999999996E-2</v>
+          </cell>
+          <cell r="G9">
+            <v>3.2656999999999985E-2</v>
+          </cell>
+          <cell r="H9">
+            <v>3.6670000000000008E-2</v>
+          </cell>
+          <cell r="I9">
+            <v>0.10956999999999997</v>
+          </cell>
+          <cell r="J9">
+            <v>6.6940000000000013E-2</v>
+          </cell>
+          <cell r="K9">
+            <v>0.10956999999999997</v>
+          </cell>
+          <cell r="L9">
+            <v>0.19170000000000006</v>
+          </cell>
+          <cell r="M9">
+            <v>0.35800999999999999</v>
+          </cell>
+          <cell r="N9">
+            <v>0.68367</v>
+          </cell>
+          <cell r="O9">
+            <v>1.2691699999999995</v>
+          </cell>
+          <cell r="P9">
+            <v>2.6727299999999992</v>
+          </cell>
+          <cell r="Q9">
+            <v>5.2848900000000008</v>
+          </cell>
+          <cell r="R9">
+            <v>5.5413700000000006</v>
+          </cell>
+          <cell r="S9">
+            <v>10.123900000000003</v>
+          </cell>
+          <cell r="T9">
+            <v>20.651010230000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="9">
+          <cell r="B9">
+            <v>1.4790000000000001E-2</v>
+          </cell>
+          <cell r="C9">
+            <v>1.4699999999999996E-2</v>
+          </cell>
+          <cell r="D9">
+            <v>1.5049999999999994E-2</v>
+          </cell>
+          <cell r="E9">
+            <v>1.4839999999999996E-2</v>
+          </cell>
+          <cell r="F9">
+            <v>1.4659999999999998E-2</v>
+          </cell>
+          <cell r="G9">
+            <v>1.6629999999999995E-2</v>
+          </cell>
+          <cell r="H9">
+            <v>1.9139999999999994E-2</v>
+          </cell>
+          <cell r="I9">
+            <v>2.6519999999999991E-2</v>
+          </cell>
+          <cell r="J9">
+            <v>3.8649999999999969E-2</v>
+          </cell>
+          <cell r="K9">
+            <v>6.3469999999999985E-2</v>
+          </cell>
+          <cell r="L9">
+            <v>0.11298000000000007</v>
+          </cell>
+          <cell r="M9">
+            <v>0.21199999999999983</v>
+          </cell>
+          <cell r="N9">
+            <v>0.41116999999999981</v>
+          </cell>
+          <cell r="O9">
+            <v>0.81407999999999991</v>
+          </cell>
+          <cell r="P9">
+            <v>1.5812099999999989</v>
+          </cell>
+          <cell r="Q9">
+            <v>3.1228600000000011</v>
+          </cell>
+          <cell r="R9">
+            <v>6.2702000000000009</v>
+          </cell>
+          <cell r="S9">
+            <v>12.519739999999999</v>
+          </cell>
+          <cell r="T9">
+            <v>25.168320019999996</v>
+          </cell>
+          <cell r="U9">
+            <v>51.016309960000015</v>
+          </cell>
+          <cell r="V9">
+            <v>102.45390990999998</v>
+          </cell>
+          <cell r="W9">
+            <v>205.31741943999995</v>
+          </cell>
+          <cell r="X9">
+            <v>412.1913299900001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="9">
+          <cell r="B9">
+            <v>1.9709999999999991E-2</v>
+          </cell>
+          <cell r="C9">
+            <v>1.9099999999999989E-2</v>
+          </cell>
+          <cell r="D9">
+            <v>1.9949999999999982E-2</v>
+          </cell>
+          <cell r="E9">
+            <v>1.9409999999999986E-2</v>
+          </cell>
+          <cell r="F9">
+            <v>1.9089999999999992E-2</v>
+          </cell>
+          <cell r="G9">
+            <v>2.2239999999999975E-2</v>
+          </cell>
+          <cell r="H9">
+            <v>2.6419999999999968E-2</v>
+          </cell>
+          <cell r="I9">
+            <v>3.6890000000000006E-2</v>
+          </cell>
+          <cell r="J9">
+            <v>5.4399999999999969E-2</v>
+          </cell>
+          <cell r="K9">
+            <v>8.8710000000000039E-2</v>
+          </cell>
+          <cell r="L9">
+            <v>0.16</v>
+          </cell>
+          <cell r="M9">
+            <v>0.30190999999999979</v>
+          </cell>
+          <cell r="N9">
+            <v>0.58777000000000035</v>
+          </cell>
+          <cell r="O9">
+            <v>1.1417200000000001</v>
+          </cell>
+          <cell r="P9">
+            <v>2.2941399999999996</v>
+          </cell>
+          <cell r="Q9">
+            <v>4.5464499999999983</v>
+          </cell>
+          <cell r="R9">
+            <v>9.0558300000000038</v>
+          </cell>
+          <cell r="S9">
+            <v>18.160590089999999</v>
+          </cell>
+          <cell r="T9">
+            <v>36.537869999999984</v>
+          </cell>
+          <cell r="U9">
+            <v>73.476889779999951</v>
+          </cell>
+          <cell r="V9">
+            <v>147.25069986000003</v>
+          </cell>
+          <cell r="W9">
+            <v>294.9716695699999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="9">
+          <cell r="B9">
+            <v>2.0779999999999989E-2</v>
+          </cell>
+          <cell r="C9">
+            <v>2.0369999999999996E-2</v>
+          </cell>
+          <cell r="D9">
+            <v>1.990999999999999E-2</v>
+          </cell>
+          <cell r="E9">
+            <v>1.9979999999999998E-2</v>
+          </cell>
+          <cell r="F9">
+            <v>1.9790000000000002E-2</v>
+          </cell>
+          <cell r="G9">
+            <v>2.0039999999999992E-2</v>
+          </cell>
+          <cell r="H9">
+            <v>2.0569999999999991E-2</v>
+          </cell>
+          <cell r="I9">
+            <v>2.2609999999999984E-2</v>
+          </cell>
+          <cell r="J9">
+            <v>2.8690000000000011E-2</v>
+          </cell>
+          <cell r="K9">
+            <v>3.6999999999999984E-2</v>
+          </cell>
+          <cell r="L9">
+            <v>5.4009999999999996E-2</v>
+          </cell>
+          <cell r="M9">
+            <v>9.0509999999999979E-2</v>
+          </cell>
+          <cell r="N9">
+            <v>0.16283000000000006</v>
+          </cell>
+          <cell r="O9">
+            <v>0.30843999999999983</v>
+          </cell>
+          <cell r="P9">
+            <v>0.58264999999999989</v>
+          </cell>
+          <cell r="Q9">
+            <v>1.1656700000000002</v>
+          </cell>
+          <cell r="R9">
+            <v>2.303879999999999</v>
+          </cell>
+          <cell r="S9">
+            <v>4.5803000000000011</v>
+          </cell>
+          <cell r="T9">
+            <v>9.1295700000000028</v>
+          </cell>
+          <cell r="U9">
+            <v>18.454040150000004</v>
+          </cell>
+          <cell r="V9">
+            <v>37.025059740000017</v>
+          </cell>
+          <cell r="W9">
+            <v>74.142030670000025</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9826,8 +12763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10:T109"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -59442,8 +62379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E31:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J119" workbookViewId="0">
-      <selection activeCell="Y134" sqref="Y134"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="AE149" sqref="AE149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>